<commit_message>
add DOI to excel file
</commit_message>
<xml_diff>
--- a/import/data_import/PN000009 Markerless Prospective Motion Correction/record_rawData.xlsx
+++ b/import/data_import/PN000009 Markerless Prospective Motion Correction/record_rawData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\data_import\MarkerlessProspectiveMoCo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PublicnEUro\DataCatalogue\import\data_import\PN000009 Markerless Prospective Motion Correction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B060AC-A610-4F23-B0C0-97BB1D058C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74115D8-68F0-44EA-92B3-05C33DF338AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="599" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -325,7 +325,7 @@
     <t>PN000009</t>
   </si>
   <si>
-    <t>10.70883/QHMG1117</t>
+    <t>https://doi.org/10.70883/QHMG1117</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1232,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="55.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1581,7 +1581,7 @@
     <hyperlink ref="B16" r:id="rId5" xr:uid="{042E520D-DC3A-465C-A1A0-E0407B43AE55}"/>
     <hyperlink ref="B7" r:id="rId6" location="dataset_descriptionjson" xr:uid="{F6C4DD7F-BDF1-415D-A415-DE85F43495B0}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{FC9DB523-70D6-417A-B2D7-B4597C9DE102}"/>
-    <hyperlink ref="C23" r:id="rId8" display="https://doi.org/1070883/QHMG1117" xr:uid="{CE0083BD-3B13-4424-9C3E-3E683DA32B28}"/>
+    <hyperlink ref="C23" r:id="rId8" xr:uid="{CE0083BD-3B13-4424-9C3E-3E683DA32B28}"/>
   </hyperlinks>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>